<commit_message>
updated CV and teaching
</commit_message>
<xml_diff>
--- a/static/files/Formidling.xlsx
+++ b/static/files/Formidling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/st06810/Dropbox/UiB/blog/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47293BE9-FBD7-C240-B9C2-774CF8242C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422E505C-F12E-5740-A000-860E185DAAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="1700" windowWidth="41940" windowHeight="22100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2017'!$A$2:$AD$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Ark2'!$B$1:$I$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Ark2'!$B$1:$I$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="343">
   <si>
     <t>p</t>
   </si>
@@ -1068,6 +1068,15 @@
   </si>
   <si>
     <t>UoB</t>
+  </si>
+  <si>
+    <t>Hvordan kan lav inntekt påvirke barns helse og utvikling?</t>
+  </si>
+  <si>
+    <t>0-24 satsingen i Trøndelag</t>
+  </si>
+  <si>
+    <t>Statsforvalter i Trøndelag</t>
   </si>
 </sst>
 </file>
@@ -4724,10 +4733,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4770,94 +4779,94 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>56</v>
+      </c>
+      <c r="B2">
+        <v>2021</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G2" t="s">
+        <v>332</v>
+      </c>
+      <c r="H2" t="s">
+        <v>342</v>
+      </c>
+      <c r="I2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>55</v>
+      </c>
+      <c r="B3">
+        <v>2021</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" t="s">
+        <v>329</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>301</v>
+      </c>
+      <c r="I3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>54</v>
       </c>
-      <c r="B2">
+      <c r="B4">
         <v>2020</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C4" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E4" t="s">
         <v>330</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F4" t="s">
         <v>329</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H4" t="s">
         <v>301</v>
       </c>
-      <c r="I2">
+      <c r="I4">
         <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
-        <v>53</v>
-      </c>
-      <c r="B3" s="19">
-        <v>2020</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>334</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>332</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="I3" s="19">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="19">
-        <v>52</v>
-      </c>
-      <c r="B4" s="19">
-        <v>2020</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>336</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>332</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="I4" s="19">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B5" s="19">
         <v>2020</v>
@@ -4872,195 +4881,195 @@
         <v>333</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H5" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="I5" s="19">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="19">
+        <v>52</v>
+      </c>
+      <c r="B6" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="I6" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="19">
+        <v>51</v>
+      </c>
+      <c r="B7" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="I5" s="19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>2020</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>293</v>
-      </c>
-      <c r="E6" t="s">
-        <v>330</v>
-      </c>
-      <c r="F6" t="s">
-        <v>329</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>301</v>
-      </c>
-      <c r="I6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>49</v>
-      </c>
-      <c r="B7">
-        <v>2020</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="E7" t="s">
-        <v>326</v>
-      </c>
-      <c r="F7" t="s">
-        <v>327</v>
-      </c>
-      <c r="G7" t="s">
-        <v>332</v>
-      </c>
-      <c r="H7" t="s">
-        <v>328</v>
-      </c>
-      <c r="I7">
+      <c r="I7" s="19">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B8">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>246</v>
+        <v>293</v>
       </c>
       <c r="E8" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="F8" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="G8" t="s">
-        <v>332</v>
+        <v>22</v>
       </c>
       <c r="H8" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E9" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F9" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="G9" t="s">
         <v>332</v>
       </c>
       <c r="H9" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="I9">
-        <v>150</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>2019</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>316</v>
+        <v>269</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>310</v>
+        <v>246</v>
       </c>
       <c r="E10" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="F10" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>332</v>
       </c>
       <c r="H10" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="I10">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>2019</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>316</v>
+        <v>269</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>310</v>
+        <v>246</v>
       </c>
       <c r="E11" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="F11" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="G11" t="s">
         <v>332</v>
       </c>
       <c r="H11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I11">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>2019</v>
@@ -5072,517 +5081,517 @@
         <v>310</v>
       </c>
       <c r="E12" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="F12" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="G12" t="s">
-        <v>332</v>
+        <v>22</v>
       </c>
       <c r="H12" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="I12">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>2019</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>262</v>
+        <v>316</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>252</v>
+        <v>310</v>
       </c>
       <c r="E13" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="F13" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="G13" t="s">
         <v>332</v>
       </c>
       <c r="H13" t="s">
-        <v>301</v>
+        <v>325</v>
       </c>
       <c r="I13">
-        <v>1200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>2019</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>266</v>
+        <v>316</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>251</v>
+        <v>310</v>
       </c>
       <c r="E14" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="F14" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="G14" t="s">
         <v>332</v>
       </c>
       <c r="H14" t="s">
-        <v>303</v>
+        <v>319</v>
       </c>
       <c r="I14">
-        <v>350</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>2019</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>291</v>
+        <v>252</v>
       </c>
       <c r="E15" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F15" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="G15" t="s">
         <v>332</v>
       </c>
       <c r="H15" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I15">
-        <v>150</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>2019</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>291</v>
+        <v>251</v>
       </c>
       <c r="E16" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="F16" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>332</v>
       </c>
       <c r="H16" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I16">
-        <v>30</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>2019</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>255</v>
+        <v>291</v>
       </c>
       <c r="E17" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>299</v>
       </c>
       <c r="G17" t="s">
         <v>332</v>
       </c>
       <c r="H17" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="I17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B18">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>287</v>
+        <v>291</v>
+      </c>
+      <c r="E18" t="s">
+        <v>330</v>
+      </c>
+      <c r="F18" t="s">
+        <v>329</v>
       </c>
       <c r="G18" t="s">
-        <v>332</v>
+        <v>22</v>
       </c>
       <c r="H18" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="I18">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>284</v>
+        <v>255</v>
+      </c>
+      <c r="E19" t="s">
+        <v>308</v>
+      </c>
+      <c r="F19" t="s">
+        <v>106</v>
       </c>
       <c r="G19" t="s">
         <v>332</v>
       </c>
       <c r="H19" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="I19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="20" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>2018</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E20" t="s">
-        <v>281</v>
-      </c>
-      <c r="F20" t="s">
-        <v>282</v>
+        <v>244</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>287</v>
       </c>
       <c r="G20" t="s">
-        <v>22</v>
+        <v>332</v>
       </c>
       <c r="H20" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="I20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>2018</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>291</v>
-      </c>
-      <c r="E21" t="s">
-        <v>278</v>
-      </c>
-      <c r="F21" t="s">
-        <v>279</v>
+        <v>252</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>284</v>
       </c>
       <c r="G21" t="s">
         <v>332</v>
       </c>
       <c r="H21" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="I21">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B22">
         <v>2018</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>247</v>
+        <v>147</v>
       </c>
       <c r="E22" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="F22" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="G22" t="s">
-        <v>332</v>
+        <v>22</v>
       </c>
       <c r="H22" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="I22">
-        <v>150</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>2018</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="E23" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F23" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="G23" t="s">
         <v>332</v>
       </c>
       <c r="H23" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="I23">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>2018</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>292</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>258</v>
+        <v>247</v>
+      </c>
+      <c r="E24" t="s">
+        <v>274</v>
       </c>
       <c r="F24" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="G24" t="s">
         <v>332</v>
       </c>
       <c r="H24" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="I24">
-        <v>235</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B25">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E25" t="s">
-        <v>210</v>
+        <v>275</v>
       </c>
       <c r="F25" t="s">
-        <v>212</v>
+        <v>276</v>
       </c>
       <c r="G25" t="s">
         <v>332</v>
       </c>
       <c r="H25" t="s">
-        <v>211</v>
+        <v>277</v>
       </c>
       <c r="I25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B26">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="E26" t="s">
-        <v>295</v>
+        <v>292</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>258</v>
       </c>
       <c r="F26" t="s">
-        <v>195</v>
+        <v>259</v>
       </c>
       <c r="G26" t="s">
         <v>332</v>
       </c>
       <c r="H26" t="s">
-        <v>114</v>
+        <v>260</v>
       </c>
       <c r="I26">
-        <v>20</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B27">
         <v>2017</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>147</v>
+        <v>252</v>
       </c>
       <c r="E27" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F27" t="s">
-        <v>189</v>
+        <v>212</v>
       </c>
       <c r="G27" t="s">
         <v>332</v>
       </c>
       <c r="H27" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="I27">
-        <v>130</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>2017</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E28" t="s">
-        <v>179</v>
+        <v>295</v>
       </c>
       <c r="F28" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="G28" t="s">
         <v>332</v>
       </c>
       <c r="H28" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="I28">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>2017</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>255</v>
+        <v>147</v>
       </c>
       <c r="E29" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F29" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G29" t="s">
         <v>332</v>
       </c>
       <c r="H29" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="I29">
-        <v>70</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>2017</v>
@@ -5594,24 +5603,24 @@
         <v>255</v>
       </c>
       <c r="E30" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F30" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G30" t="s">
         <v>332</v>
       </c>
       <c r="H30" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
       <c r="I30">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B31">
         <v>2017</v>
@@ -5623,82 +5632,82 @@
         <v>255</v>
       </c>
       <c r="E31" t="s">
-        <v>257</v>
+        <v>183</v>
       </c>
       <c r="F31" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="G31" t="s">
         <v>332</v>
       </c>
       <c r="H31" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="I31">
-        <v>120</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B32">
         <v>2017</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>292</v>
+        <v>255</v>
       </c>
       <c r="E32" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="F32" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="G32" t="s">
-        <v>22</v>
+        <v>332</v>
       </c>
       <c r="H32" t="s">
-        <v>34</v>
+        <v>114</v>
       </c>
       <c r="I32">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B33">
         <v>2017</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>292</v>
+        <v>255</v>
       </c>
       <c r="E33" t="s">
-        <v>162</v>
+        <v>257</v>
       </c>
       <c r="F33" t="s">
-        <v>235</v>
+        <v>172</v>
       </c>
       <c r="G33" t="s">
         <v>332</v>
       </c>
       <c r="H33" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="I33">
-        <v>370</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B34">
         <v>2017</v>
@@ -5710,271 +5719,271 @@
         <v>292</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="F34" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="G34" t="s">
-        <v>332</v>
+        <v>22</v>
       </c>
       <c r="H34" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="I34">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B35">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>246</v>
+        <v>292</v>
       </c>
       <c r="E35" t="s">
-        <v>296</v>
+        <v>162</v>
       </c>
       <c r="F35" t="s">
-        <v>98</v>
+        <v>235</v>
       </c>
       <c r="G35" t="s">
         <v>332</v>
       </c>
       <c r="H35" t="s">
-        <v>97</v>
+        <v>163</v>
       </c>
       <c r="I35">
-        <v>7</v>
+        <v>370</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B36">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>252</v>
+        <v>292</v>
       </c>
       <c r="E36" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="F36" t="s">
-        <v>237</v>
+        <v>160</v>
       </c>
       <c r="G36" t="s">
         <v>332</v>
       </c>
       <c r="H36" t="s">
-        <v>140</v>
+        <v>50</v>
       </c>
       <c r="I36">
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B37">
         <v>2016</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E37" t="s">
-        <v>118</v>
+        <v>296</v>
       </c>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="G37" t="s">
         <v>332</v>
       </c>
       <c r="H37" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="I37">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B38">
         <v>2016</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>293</v>
+        <v>252</v>
       </c>
       <c r="E38" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F38" t="s">
-        <v>155</v>
+        <v>237</v>
       </c>
       <c r="G38" t="s">
         <v>332</v>
       </c>
       <c r="H38" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="I38">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B39">
         <v>2016</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E39" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="F39" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="G39" t="s">
         <v>332</v>
       </c>
       <c r="H39" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="I39">
-        <v>150</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B40">
         <v>2016</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>251</v>
+        <v>293</v>
       </c>
       <c r="E40" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="F40" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="G40" t="s">
         <v>332</v>
       </c>
       <c r="H40" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="I40">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B41">
         <v>2016</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>291</v>
+        <v>249</v>
       </c>
       <c r="E41" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="F41" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="G41" t="s">
         <v>332</v>
       </c>
       <c r="H41" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I41">
-        <v>70</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B42">
         <v>2016</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>291</v>
+        <v>251</v>
       </c>
       <c r="E42" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="F42" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G42" t="s">
         <v>332</v>
       </c>
       <c r="H42" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="I42">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B43">
         <v>2016</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>127</v>
       </c>
       <c r="F43" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="G43" t="s">
         <v>332</v>
@@ -5988,22 +5997,22 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B44">
         <v>2016</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="E44" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F44" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="G44" t="s">
         <v>332</v>
@@ -6012,70 +6021,70 @@
         <v>50</v>
       </c>
       <c r="I44">
-        <v>300</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B45">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E45" t="s">
-        <v>297</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="G45" t="s">
         <v>332</v>
       </c>
       <c r="H45" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="I45">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B46">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E46" t="s">
-        <v>297</v>
+        <v>101</v>
       </c>
       <c r="F46" t="s">
-        <v>239</v>
+        <v>102</v>
       </c>
       <c r="G46" t="s">
-        <v>22</v>
+        <v>332</v>
       </c>
       <c r="H46" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="I46">
-        <v>30</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B47">
         <v>2015</v>
@@ -6087,16 +6096,16 @@
         <v>246</v>
       </c>
       <c r="E47" t="s">
-        <v>16</v>
+        <v>297</v>
       </c>
       <c r="F47" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="G47" t="s">
         <v>332</v>
       </c>
       <c r="H47" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="I47">
         <v>100</v>
@@ -6104,51 +6113,51 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B48">
         <v>2015</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E48" t="s">
-        <v>52</v>
+        <v>297</v>
       </c>
       <c r="F48" t="s">
-        <v>53</v>
+        <v>239</v>
       </c>
       <c r="G48" t="s">
-        <v>332</v>
+        <v>22</v>
       </c>
       <c r="H48" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="I48">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B49">
         <v>2015</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E49" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="F49" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="G49" t="s">
         <v>332</v>
@@ -6157,12 +6166,12 @@
         <v>50</v>
       </c>
       <c r="I49">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B50">
         <v>2015</v>
@@ -6174,170 +6183,228 @@
         <v>244</v>
       </c>
       <c r="E50" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F50" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G50" t="s">
         <v>332</v>
       </c>
       <c r="H50" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="I50">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B51">
         <v>2015</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E51" t="s">
-        <v>298</v>
+        <v>48</v>
       </c>
       <c r="F51" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="G51" t="s">
         <v>332</v>
       </c>
       <c r="H51" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="I51">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B52">
         <v>2015</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>147</v>
+        <v>244</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F52" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G52" t="s">
         <v>332</v>
       </c>
       <c r="H52" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="I52">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B53">
         <v>2015</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E53" t="s">
-        <v>21</v>
+        <v>298</v>
       </c>
       <c r="F53" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G53" t="s">
-        <v>22</v>
+        <v>332</v>
       </c>
       <c r="H53" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I53">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B54">
         <v>2015</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>292</v>
+        <v>147</v>
       </c>
       <c r="E54" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F54" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G54" t="s">
         <v>332</v>
       </c>
       <c r="H54" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="I54">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B55">
         <v>2015</v>
       </c>
       <c r="C55" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="E55" t="s">
+        <v>21</v>
+      </c>
+      <c r="F55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" t="s">
+        <v>12</v>
+      </c>
+      <c r="I55">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56">
+        <v>2015</v>
+      </c>
+      <c r="C56" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D56" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>36</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F56" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56" t="s">
+        <v>332</v>
+      </c>
+      <c r="H56" t="s">
         <v>37</v>
       </c>
-      <c r="G55" t="s">
+      <c r="I56">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>2015</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="E57" t="s">
+        <v>36</v>
+      </c>
+      <c r="F57" t="s">
+        <v>37</v>
+      </c>
+      <c r="G57" t="s">
         <v>332</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H57" t="s">
         <v>40</v>
       </c>
-      <c r="I55">
+      <c r="I57">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I55" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:I65">
-    <sortCondition descending="1" ref="A6:A65"/>
+  <autoFilter ref="B1:I57" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:I67">
+    <sortCondition descending="1" ref="A8:A67"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>